<commit_message>
updateID89 and ID83 mapping. Update introduction
</commit_message>
<xml_diff>
--- a/ID89.signature.summary/ID89_and_ID83.summary.xlsx
+++ b/ID89.signature.summary/ID89_and_ID83.summary.xlsx
@@ -5,16 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmliu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9c7212a1ac174da/文档/GitHub/Liu2024/ID89.signature.summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BEEB8B0-F78B-411B-9460-2F95DE12C071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{5BEEB8B0-F78B-411B-9460-2F95DE12C071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F699943-9647-46E1-91CD-1FF36E5EF591}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18912" windowHeight="11952" xr2:uid="{1EAECB79-A789-42D9-86BA-9215C29F9749}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1EAECB79-A789-42D9-86BA-9215C29F9749}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$B$3:$B$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="164">
   <si>
     <t>ID89 name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -481,6 +486,177 @@
   </si>
   <si>
     <t>MSI. Consistent with Serena's finding.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InD1</t>
+  </si>
+  <si>
+    <t>InD2a</t>
+  </si>
+  <si>
+    <t>InD2b</t>
+  </si>
+  <si>
+    <t>InD3a</t>
+  </si>
+  <si>
+    <t>InD3b</t>
+  </si>
+  <si>
+    <t>InD4a</t>
+  </si>
+  <si>
+    <t>InD4b</t>
+  </si>
+  <si>
+    <t>InD5</t>
+  </si>
+  <si>
+    <t>InD6</t>
+  </si>
+  <si>
+    <t>InD7</t>
+  </si>
+  <si>
+    <t>InD8</t>
+  </si>
+  <si>
+    <t>InD9a</t>
+  </si>
+  <si>
+    <t>InD9b</t>
+  </si>
+  <si>
+    <t>InD9c</t>
+  </si>
+  <si>
+    <t>InD10</t>
+  </si>
+  <si>
+    <t>InD11</t>
+  </si>
+  <si>
+    <t>InD12</t>
+  </si>
+  <si>
+    <t>InD13</t>
+  </si>
+  <si>
+    <t>InD14</t>
+  </si>
+  <si>
+    <t>InD15</t>
+  </si>
+  <si>
+    <t>InD16a</t>
+  </si>
+  <si>
+    <t>InD16b</t>
+  </si>
+  <si>
+    <t>InD18</t>
+  </si>
+  <si>
+    <t>InD19</t>
+  </si>
+  <si>
+    <t>InD20</t>
+  </si>
+  <si>
+    <t>InD21</t>
+  </si>
+  <si>
+    <t>InD23</t>
+  </si>
+  <si>
+    <t>InD24</t>
+  </si>
+  <si>
+    <t>InD26</t>
+  </si>
+  <si>
+    <t>InD27</t>
+  </si>
+  <si>
+    <t>InD28</t>
+  </si>
+  <si>
+    <t>InD28m</t>
+  </si>
+  <si>
+    <t>InD29</t>
+  </si>
+  <si>
+    <t>InD30</t>
+  </si>
+  <si>
+    <t>InD31</t>
+  </si>
+  <si>
+    <t>InD32</t>
+  </si>
+  <si>
+    <t>InD33</t>
+  </si>
+  <si>
+    <t>no sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">artefact </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Similar to InD26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.913 cosine to InD26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>similar to InD2a 0.90</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>difference only driven by two peaks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InsDel3 average the ratio between insT and del T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InD20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">cosine </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InD16a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InD16b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>merged</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InD11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InD9c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InsDel4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -488,7 +664,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,16 +680,346 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线 Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="4"/>
+      <color rgb="FF586E75"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDF6E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -521,19 +1027,226 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1 2" xfId="20" xr:uid="{96642AB3-9DEB-44DC-BE63-718714B165A9}"/>
+    <cellStyle name="20% - Accent2 2" xfId="24" xr:uid="{8CA25984-6049-4CC1-874A-4CD1DCF11BEB}"/>
+    <cellStyle name="20% - Accent3 2" xfId="28" xr:uid="{F88C8642-35AD-44AC-9C97-5C9879AED1D9}"/>
+    <cellStyle name="20% - Accent4 2" xfId="32" xr:uid="{B9A7130C-2B7B-413E-B2FB-0B22BB4A5620}"/>
+    <cellStyle name="20% - Accent5 2" xfId="36" xr:uid="{039EB24F-2071-4414-AAF6-71E3992C4D64}"/>
+    <cellStyle name="20% - Accent6 2" xfId="40" xr:uid="{0FBC6884-1F53-4128-883F-9B8BCE1807A4}"/>
+    <cellStyle name="40% - Accent1 2" xfId="21" xr:uid="{81A7911C-11E1-4D48-AE21-D6FEE97327C6}"/>
+    <cellStyle name="40% - Accent2 2" xfId="25" xr:uid="{792D4FA8-F361-4B89-9648-B11E4AB6FEE6}"/>
+    <cellStyle name="40% - Accent3 2" xfId="29" xr:uid="{F3A43A05-7446-4F28-AC0E-B2A1931D310B}"/>
+    <cellStyle name="40% - Accent4 2" xfId="33" xr:uid="{50F1DBCE-D2BB-4193-8729-F28BAF20E904}"/>
+    <cellStyle name="40% - Accent5 2" xfId="37" xr:uid="{6BB88AD7-4798-47ED-A17F-98F5648189B1}"/>
+    <cellStyle name="40% - Accent6 2" xfId="41" xr:uid="{B4D55D85-6812-4E20-BA88-FCAFA1B472BA}"/>
+    <cellStyle name="60% - Accent1 2" xfId="22" xr:uid="{B5FFAC1A-6C7D-44DE-842B-DD0287DA5FB6}"/>
+    <cellStyle name="60% - Accent2 2" xfId="26" xr:uid="{26D2CF15-340F-4953-B39D-1130C77063F5}"/>
+    <cellStyle name="60% - Accent3 2" xfId="30" xr:uid="{AFA8058D-F5FF-42EE-A6E4-7C1B4A308F62}"/>
+    <cellStyle name="60% - Accent4 2" xfId="34" xr:uid="{B5ACDDAF-812F-4464-9328-4B9AB3A2E6B5}"/>
+    <cellStyle name="60% - Accent5 2" xfId="38" xr:uid="{E96CABD5-076F-4081-A4A0-C6683F9A7F9A}"/>
+    <cellStyle name="60% - Accent6 2" xfId="42" xr:uid="{428C22BE-5C18-4E53-A2D6-16CA1996AF06}"/>
+    <cellStyle name="Accent1 2" xfId="19" xr:uid="{E24681E1-6199-421E-9C13-5EFC2E594260}"/>
+    <cellStyle name="Accent2 2" xfId="23" xr:uid="{6A7C99C8-A46D-4FFA-AD93-55D9A9E6414E}"/>
+    <cellStyle name="Accent3 2" xfId="27" xr:uid="{E38DEF6C-5D7C-439A-90DF-383FE9490E0F}"/>
+    <cellStyle name="Accent4 2" xfId="31" xr:uid="{0D742E24-16F8-4364-8B75-EC417582CD35}"/>
+    <cellStyle name="Accent5 2" xfId="35" xr:uid="{3B368C49-53A4-481A-AFC9-13B4FCE79F25}"/>
+    <cellStyle name="Accent6 2" xfId="39" xr:uid="{F0E833EA-D37A-4872-82AC-39F839F66266}"/>
+    <cellStyle name="Bad 2" xfId="8" xr:uid="{A5B94227-7015-4DC8-94B4-0F4B98F553AF}"/>
+    <cellStyle name="Calculation 2" xfId="12" xr:uid="{7EC537D9-AC70-4678-95DD-537F07D054B1}"/>
+    <cellStyle name="Check Cell 2" xfId="14" xr:uid="{3A39C4D7-9808-4EC2-844E-CD8E1E93607D}"/>
+    <cellStyle name="Explanatory Text 2" xfId="17" xr:uid="{8CAECE8C-4043-4DD9-B5B0-EB563A50873C}"/>
+    <cellStyle name="Good 2" xfId="7" xr:uid="{9E3960AD-357B-4E71-BE37-D53A6D87360A}"/>
+    <cellStyle name="Heading 1 2" xfId="3" xr:uid="{39C7DA6F-562D-4DFE-A1C2-8571745C4132}"/>
+    <cellStyle name="Heading 2 2" xfId="4" xr:uid="{3229B593-04A0-49A9-B759-C98E9CF2667F}"/>
+    <cellStyle name="Heading 3 2" xfId="5" xr:uid="{198F7BC9-9C5B-45AF-BA6D-2F53E8C564B9}"/>
+    <cellStyle name="Heading 4 2" xfId="6" xr:uid="{607A85DD-B84C-41B7-A0AE-4378BE91304A}"/>
+    <cellStyle name="Input 2" xfId="10" xr:uid="{64AAD20E-15D7-4B27-9413-58598874AD3B}"/>
+    <cellStyle name="Linked Cell 2" xfId="13" xr:uid="{4C20ECC6-9763-4CFF-9C8C-2F1B5423E4C4}"/>
+    <cellStyle name="Neutral 2" xfId="9" xr:uid="{147B04D1-63EF-48A4-9314-A91DB37A2B5F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{C9FCF362-AD1D-469A-A8DA-C087233CA890}"/>
+    <cellStyle name="Note 2" xfId="16" xr:uid="{4D2508C8-D9E3-4B1E-A44D-634E7E18D427}"/>
+    <cellStyle name="Output 2" xfId="11" xr:uid="{D91CBB14-3612-4788-93E4-587005D23398}"/>
+    <cellStyle name="Title 2" xfId="2" xr:uid="{439C42B8-5714-4931-9587-5840C9E6640A}"/>
+    <cellStyle name="Total 2" xfId="18" xr:uid="{DFAF6DCB-5D51-41E5-B93C-2BFA1AEF769F}"/>
+    <cellStyle name="Warning Text 2" xfId="15" xr:uid="{4D7BDAD1-7788-4BDD-9A83-A6B54C400D77}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -847,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1986EDA-ED44-411B-A31B-549A3D83E29F}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -1373,4 +2086,534 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A609C6E4-D419-4D76-BEA7-70168B835FEF}">
+  <dimension ref="A1:AK37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:37" ht="15" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E60368-785E-4116-BD49-B69E31273F1D}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B2">
+        <v>0.43030590000000002</v>
+      </c>
+      <c r="C2">
+        <v>0.12941359999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.44028050000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B4">
+        <v>0.54020354000000004</v>
+      </c>
+      <c r="C4">
+        <v>0.37409509000000002</v>
+      </c>
+      <c r="D4">
+        <v>8.5701319999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B6">
+        <v>0.48259819999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.27442290000000003</v>
+      </c>
+      <c r="D6">
+        <v>0.2429789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B8">
+        <v>0.56460290000000002</v>
+      </c>
+      <c r="C8">
+        <v>0.43539709999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B10">
+        <v>0.2068497</v>
+      </c>
+      <c r="C10">
+        <v>0.37033830000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.42281200000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>0.90700000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B12">
+        <v>0.22818150000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.77181840000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>